<commit_message>
change name and bed 300k
- All Scenario A change maximum number of hospital surge beds to 300,000
- change format of plotting
ex.
"Eff1_A_high_inc_70_1year" to "70% VE (severity), 1 year duration, HT group"
</commit_message>
<xml_diff>
--- a/Scenario_A/CoMo doc/TH_CoMoCOVID_severity_A_high_inc_70_1year.xlsx
+++ b/Scenario_A/CoMo doc/TH_CoMoCOVID_severity_A_high_inc_70_1year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\como\wave1_2022\Scenario_A\severity_A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanaphum\Documents\GitHub\CoVac19TH\Scenario_A\CoMo doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178F2301-8307-426B-B17D-8444B79A519B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B0231-D0F0-4AB3-A781-9F7DBBF14DF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" tabRatio="648" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" tabRatio="648" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -4057,18 +4057,18 @@
       <sheetName val="HIDDEN"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
       <sheetData sheetId="12">
         <row r="2">
           <cell r="E2" t="str">
@@ -18723,8 +18723,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -18759,7 +18759,7 @@
         <v>186</v>
       </c>
       <c r="B2" s="72">
-        <v>177292</v>
+        <v>300000</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>187</v>
@@ -19140,7 +19140,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>